<commit_message>
support importing of doubles entries
</commit_message>
<xml_diff>
--- a/testdata/Mens Doubles.xlsx
+++ b/testdata/Mens Doubles.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14360" activeTab="1"/>
+    <workbookView windowHeight="15660"/>
   </bookViews>
   <sheets>
     <sheet name="entries" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="38">
   <si>
     <t>SN</t>
   </si>
@@ -51,6 +51,9 @@
     <t>Wang Chuqin</t>
   </si>
   <si>
+    <t>CHN</t>
+  </si>
+  <si>
     <t>Ma Long</t>
   </si>
   <si>
@@ -75,6 +78,9 @@
     <t>Truls Moregard</t>
   </si>
   <si>
+    <t>EUR</t>
+  </si>
+  <si>
     <t>Darko Jorgic</t>
   </si>
   <si>
@@ -85,6 +91,9 @@
   </si>
   <si>
     <t>Jang Woojin</t>
+  </si>
+  <si>
+    <t>KOR</t>
   </si>
   <si>
     <t>Quadri Aruna</t>
@@ -140,11 +149,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="5">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="178" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="180" formatCode="yyyy\-mm\-dd"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -607,16 +616,16 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -753,7 +762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1291,8 +1300,8 @@
   <sheetPr/>
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.8" outlineLevelCol="4"/>
@@ -1327,7 +1336,9 @@
       <c r="C2" t="s">
         <v>6</v>
       </c>
-      <c r="D2"/>
+      <c r="D2" t="s">
+        <v>7</v>
+      </c>
       <c r="E2">
         <v>1</v>
       </c>
@@ -1337,12 +1348,14 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3"/>
       <c r="E3">
         <v>2</v>
       </c>
@@ -1352,10 +1365,10 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D4"/>
       <c r="E4">
@@ -1367,47 +1380,56 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5"/>
       <c r="E5">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>15</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:4">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" t="s">
-        <v>18</v>
+        <v>20</v>
+      </c>
+      <c r="D8" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="9" spans="1:3">
@@ -1415,10 +1437,10 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:3">
@@ -1426,10 +1448,10 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -1437,10 +1459,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -1448,10 +1470,10 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -1459,10 +1481,10 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C13" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -1470,10 +1492,10 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1487,7 +1509,7 @@
   <sheetPr/>
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2:C27"/>
     </sheetView>
   </sheetViews>
@@ -1503,13 +1525,13 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="C1" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="D1" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:4">
@@ -1523,7 +1545,7 @@
         <v>36893</v>
       </c>
       <c r="D2" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1531,13 +1553,13 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C3" s="1">
         <v>36894</v>
       </c>
       <c r="D3" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1545,13 +1567,13 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C4" s="1">
         <v>36895</v>
       </c>
       <c r="D4" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1559,13 +1581,13 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C5" s="1">
         <v>36896</v>
       </c>
       <c r="D5" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1573,13 +1595,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C6" s="1">
         <v>36897</v>
       </c>
       <c r="D6" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1587,13 +1609,13 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C7" s="1">
         <v>36898</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1601,13 +1623,13 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C8" s="1">
         <v>36899</v>
       </c>
       <c r="D8" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1615,13 +1637,13 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="C9" s="1">
         <v>36900</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1629,13 +1651,13 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C10" s="1">
         <v>36901</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1643,13 +1665,13 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C11" s="1">
         <v>36902</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1657,13 +1679,13 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C12" s="1">
         <v>36903</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1671,13 +1693,13 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C13" s="1">
         <v>36904</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1685,13 +1707,13 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C14" s="1">
         <v>36905</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1705,7 +1727,7 @@
         <v>36906</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1713,13 +1735,13 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="1">
         <v>36907</v>
       </c>
       <c r="D16" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1727,13 +1749,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="1">
         <v>36908</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1741,13 +1763,13 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C18" s="1">
         <v>36909</v>
       </c>
       <c r="D18" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1755,13 +1777,13 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C19" s="1">
         <v>36910</v>
       </c>
       <c r="D19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1769,13 +1791,13 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C20" s="1">
         <v>36911</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1783,13 +1805,13 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" s="1">
         <v>36912</v>
       </c>
       <c r="D21" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1797,13 +1819,13 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C22" s="1">
         <v>36913</v>
       </c>
       <c r="D22" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1811,13 +1833,13 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C23" s="1">
         <v>36914</v>
       </c>
       <c r="D23" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1825,13 +1847,13 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C24" s="1">
         <v>36915</v>
       </c>
       <c r="D24" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1839,13 +1861,13 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C25" s="1">
         <v>36916</v>
       </c>
       <c r="D25" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1853,13 +1875,13 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="C26" s="1">
         <v>36917</v>
       </c>
       <c r="D26" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1867,13 +1889,13 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C27" s="1">
         <v>36918</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>